<commit_message>
Fixed naming in cars excel
</commit_message>
<xml_diff>
--- a/FilteredCarsData.xlsx
+++ b/FilteredCarsData.xlsx
@@ -17,64 +17,64 @@
     <t>Car Names</t>
   </si>
   <si>
-    <t>Car price</t>
+    <t>Car Price</t>
+  </si>
+  <si>
+    <t>Honda Brio 2011-2013 Honda Brio S MT</t>
   </si>
   <si>
     <t>Rs. 3.16 Lakh</t>
   </si>
   <si>
-    <t>Honda Brio 2011-2013 Honda Brio S MT</t>
+    <t>Honda Amaze 2013-2016 Honda Amaze S AT i-Vtech</t>
   </si>
   <si>
     <t>Rs. 3.90 Lakh</t>
   </si>
   <si>
-    <t>Honda Amaze 2013-2016 Honda Amaze S AT i-Vtech</t>
-  </si>
-  <si>
     <t>Rs. 3.05 Lakh</t>
   </si>
   <si>
+    <t>Honda Brio 2013-2016 Honda Brio S MT</t>
+  </si>
+  <si>
     <t>Rs. 3.50 Lakh</t>
   </si>
   <si>
-    <t>Honda Brio 2013-2016 Honda Brio S MT</t>
-  </si>
-  <si>
     <t>Rs. 3.60 Lakh</t>
   </si>
   <si>
+    <t>Honda City 2008-2011 Honda City 1.5 S MT</t>
+  </si>
+  <si>
     <t>Rs. 4.00 Lakh</t>
   </si>
   <si>
-    <t>Honda City 2008-2011 Honda City 1.5 S MT</t>
+    <t>Honda Jazz 2014-2020 Honda Jazz 1.2 SV i VTEC</t>
   </si>
   <si>
     <t>Rs. 3.85 Lakh</t>
   </si>
   <si>
-    <t>Honda Jazz 2014-2020 Honda Jazz 1.2 SV i VTEC</t>
+    <t>Honda City ZX 2005-2008 Honda City GXi</t>
   </si>
   <si>
     <t>Rs. 2.10 Lakh</t>
   </si>
   <si>
-    <t>Honda City ZX 2005-2008 Honda City GXi</t>
-  </si>
-  <si>
     <t>Honda Amaze 2013-2016 Honda Amaze VX i-Vtech</t>
   </si>
   <si>
+    <t>Honda Civic 2010-2013 Honda Civic 1.8 V MT</t>
+  </si>
+  <si>
     <t>Rs. 3.00 Lakh</t>
   </si>
   <si>
-    <t>Honda Civic 2010-2013 Honda Civic 1.8 V MT</t>
+    <t>Honda Brio 2011-2013 Honda Brio E MT</t>
   </si>
   <si>
     <t>Rs. 1.90 Lakh</t>
-  </si>
-  <si>
-    <t>Honda Brio 2011-2013 Honda Brio E MT</t>
   </si>
 </sst>
 </file>
@@ -151,10 +151,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>6</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -167,10 +167,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>9</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -199,10 +199,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -215,10 +215,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
BDD started + code refact pages
</commit_message>
<xml_diff>
--- a/FilteredCarsData.xlsx
+++ b/FilteredCarsData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Car Names</t>
   </si>
@@ -20,6 +20,12 @@
     <t>Car Price</t>
   </si>
   <si>
+    <t>Honda Amaze 2013-2016 Honda Amaze VX AT i-Vtech</t>
+  </si>
+  <si>
+    <t>Rs. 3.90 Lakh</t>
+  </si>
+  <si>
     <t>Honda Brio 2011-2013 Honda Brio S MT</t>
   </si>
   <si>
@@ -27,9 +33,6 @@
   </si>
   <si>
     <t>Honda Amaze 2013-2016 Honda Amaze S AT i-Vtech</t>
-  </si>
-  <si>
-    <t>Rs. 3.90 Lakh</t>
   </si>
   <si>
     <t>Rs. 3.05 Lakh</t>
@@ -151,23 +154,23 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>7</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>9</v>
@@ -175,34 +178,34 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>10</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>12</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>16</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -210,23 +213,23 @@
         <v>17</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>